<commit_message>
Time is solve_pbtk is days not hours!
</commit_message>
<xml_diff>
--- a/level2table.xlsx
+++ b/level2table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\tkqsars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0674A72A-5BE4-4ACE-A959-4638626DC689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5852AF12-516F-4794-80EA-E2075498BC7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7725" yWindow="2985" windowWidth="20265" windowHeight="11520" xr2:uid="{FEAEA17A-D745-4C2D-8DD3-2C789FAB878F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FEAEA17A-D745-4C2D-8DD3-2C789FAB878F}"/>
   </bookViews>
   <sheets>
     <sheet name="Table4" sheetId="1" r:id="rId1"/>
@@ -784,23 +784,23 @@
       </c>
       <c r="E3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.95899999999999996</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="F3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.315</v>
+        <v>0.309</v>
       </c>
       <c r="G3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>0.29799999999999999</v>
+        <v>0.315</v>
       </c>
       <c r="H3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>0.49</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="I3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>0.16300000000000001</v>
+        <v>6.1800000000000001E-2</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -813,35 +813,35 @@
       </c>
       <c r="B4" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.501</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="C4" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.89700000000000002</v>
+        <v>0.83599999999999997</v>
       </c>
       <c r="D4" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>-0.106</v>
+        <v>-2.29E-2</v>
       </c>
       <c r="E4" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.38100000000000001</v>
+        <v>0.495</v>
       </c>
       <c r="F4" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.23</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="G4" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>-0.81100000000000005</v>
+        <v>3.44</v>
       </c>
       <c r="H4" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>-0.39800000000000002</v>
+        <v>6.72</v>
       </c>
       <c r="I4" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.93500000000000005</v>
+        <v>-0.46400000000000002</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -854,35 +854,35 @@
       </c>
       <c r="B5" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.60299999999999998</v>
+        <v>0.621</v>
       </c>
       <c r="C5" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.8</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="D5" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>-2.69E-2</v>
+        <v>0.15</v>
       </c>
       <c r="E5" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.54600000000000004</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="F5" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.05</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="G5" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>-0.67900000000000005</v>
+        <v>5.88</v>
       </c>
       <c r="H5" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>-0.25700000000000001</v>
+        <v>10.5</v>
       </c>
       <c r="I5" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.89200000000000002</v>
+        <v>-0.437</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -895,35 +895,35 @@
       </c>
       <c r="B6" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.53600000000000003</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="C6" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.86599999999999999</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="D6" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>-9.1899999999999996E-2</v>
+        <v>1.6899999999999998E-2</v>
       </c>
       <c r="E6" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.501</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="F6" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.1000000000000001</v>
+        <v>1.01</v>
       </c>
       <c r="G6" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>-0.82799999999999996</v>
+        <v>3.32</v>
       </c>
       <c r="H6" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>-0.64100000000000001</v>
+        <v>5</v>
       </c>
       <c r="I6" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.92700000000000005</v>
+        <v>-3.8199999999999998E-2</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -936,35 +936,35 @@
       </c>
       <c r="B7" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.505</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C7" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.89400000000000002</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="D7" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>-0.22800000000000001</v>
+        <v>-0.105</v>
       </c>
       <c r="E7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.29699999999999999</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="F7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.31</v>
+        <v>1.22</v>
       </c>
       <c r="G7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>-0.89100000000000001</v>
+        <v>2.29</v>
       </c>
       <c r="H7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>-0.48599999999999999</v>
+        <v>5.99</v>
       </c>
       <c r="I7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.97799999999999998</v>
+        <v>-0.79600000000000004</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -976,35 +976,35 @@
       </c>
       <c r="B8" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.52200000000000002</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="C8" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.878</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="D8" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>1.2E-2</v>
+        <v>0.111</v>
       </c>
       <c r="E8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.46</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.1499999999999999</v>
+        <v>1.04</v>
       </c>
       <c r="G8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>-0.71499999999999997</v>
+        <v>4.67</v>
       </c>
       <c r="H8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>-0.36599999999999999</v>
+        <v>7.93</v>
       </c>
       <c r="I8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.89300000000000002</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1016,35 +1016,35 @@
       </c>
       <c r="B9" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.377</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="C9" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>1</v>
+        <v>0.93</v>
       </c>
       <c r="D9" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>0.19</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="E9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>5.0200000000000002E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="F9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.52</v>
+        <v>1.48</v>
       </c>
       <c r="G9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>-0.78</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>-0.13800000000000001</v>
+        <v>12.1</v>
       </c>
       <c r="I9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.98199999999999998</v>
+        <v>-0.88100000000000001</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1169,7 +1169,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,13 +1193,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.501</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="C2">
-        <v>0.89700000000000002</v>
+        <v>0.83599999999999997</v>
       </c>
       <c r="D2">
-        <v>-0.106</v>
+        <v>-2.29E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1207,13 +1207,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.60299999999999998</v>
+        <v>0.621</v>
       </c>
       <c r="C3">
-        <v>0.8</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="D3">
-        <v>-2.69E-2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,13 +1221,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.53600000000000003</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="C4">
-        <v>0.86599999999999999</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="D4">
-        <v>-9.1899999999999996E-2</v>
+        <v>1.6899999999999998E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1235,13 +1235,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.505</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="C5">
-        <v>0.89400000000000002</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="D5">
-        <v>-0.22800000000000001</v>
+        <v>-0.105</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1249,13 +1249,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.52200000000000002</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="C6">
-        <v>0.878</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="D6">
-        <v>1.2E-2</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1277,13 +1277,13 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0.377</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.93</v>
       </c>
       <c r="D8">
-        <v>0.19</v>
+        <v>0.53100000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1291,13 +1291,13 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>0.53800000000000003</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="C9">
-        <v>0.93300000000000005</v>
+        <v>0.86399999999999999</v>
       </c>
       <c r="D9">
-        <v>4.1799999999999997E-2</v>
+        <v>0.156</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +1310,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B2" sqref="B2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,19 +1340,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.38100000000000001</v>
+        <v>0.495</v>
       </c>
       <c r="C2">
-        <v>1.23</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D2">
-        <v>-0.81100000000000005</v>
+        <v>3.44</v>
       </c>
       <c r="E2">
-        <v>-0.39800000000000002</v>
+        <v>6.72</v>
       </c>
       <c r="F2">
-        <v>-0.93500000000000005</v>
+        <v>-0.46400000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1360,19 +1360,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.54600000000000004</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="C3">
-        <v>1.05</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="D3">
-        <v>-0.67900000000000005</v>
+        <v>5.88</v>
       </c>
       <c r="E3">
-        <v>-0.25700000000000001</v>
+        <v>10.5</v>
       </c>
       <c r="F3">
-        <v>-0.89200000000000002</v>
+        <v>-0.437</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1380,19 +1380,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.501</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="C4">
-        <v>1.1000000000000001</v>
+        <v>1.01</v>
       </c>
       <c r="D4">
-        <v>-0.82799999999999996</v>
+        <v>3.32</v>
       </c>
       <c r="E4">
-        <v>-0.64100000000000001</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>-0.92700000000000005</v>
+        <v>-3.8199999999999998E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1400,19 +1400,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.29699999999999999</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="C5">
-        <v>1.31</v>
+        <v>1.22</v>
       </c>
       <c r="D5">
-        <v>-0.89100000000000001</v>
+        <v>2.29</v>
       </c>
       <c r="E5">
-        <v>-0.48599999999999999</v>
+        <v>5.99</v>
       </c>
       <c r="F5">
-        <v>-0.97799999999999998</v>
+        <v>-0.79600000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1420,19 +1420,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.46</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="C6">
-        <v>1.1499999999999999</v>
+        <v>1.04</v>
       </c>
       <c r="D6">
-        <v>-0.71499999999999997</v>
+        <v>4.67</v>
       </c>
       <c r="E6">
-        <v>-0.36599999999999999</v>
+        <v>7.93</v>
       </c>
       <c r="F6">
-        <v>-0.89300000000000002</v>
+        <v>0.38500000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1440,19 +1440,19 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.95899999999999996</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="C7">
+        <v>0.309</v>
+      </c>
+      <c r="D7">
         <v>0.315</v>
       </c>
-      <c r="D7">
-        <v>0.29799999999999999</v>
-      </c>
       <c r="E7">
-        <v>0.49</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="F7">
-        <v>0.16300000000000001</v>
+        <v>6.1800000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,19 +1460,19 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>5.0200000000000002E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="C8">
-        <v>1.52</v>
+        <v>1.48</v>
       </c>
       <c r="D8">
-        <v>-0.78</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E8">
-        <v>-0.13800000000000001</v>
+        <v>12.1</v>
       </c>
       <c r="F8">
-        <v>-0.98199999999999998</v>
+        <v>-0.88100000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1480,19 +1480,19 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>0.53300000000000003</v>
+        <v>0.622</v>
       </c>
       <c r="C9">
-        <v>1.2</v>
+        <v>1.08</v>
       </c>
       <c r="D9">
-        <v>-0.75</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="E9">
-        <v>-0.27200000000000002</v>
+        <v>10.5</v>
       </c>
       <c r="F9">
-        <v>-0.90800000000000003</v>
+        <v>-0.11799999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More stats for httk-measured chems
</commit_message>
<xml_diff>
--- a/level2table.xlsx
+++ b/level2table.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\tkqsars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5852AF12-516F-4794-80EA-E2075498BC7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BEDA8B-2BE4-485B-BA56-A72830782B6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FEAEA17A-D745-4C2D-8DD3-2C789FAB878F}"/>
+    <workbookView xWindow="1140" yWindow="510" windowWidth="20895" windowHeight="11955" activeTab="1" xr2:uid="{FEAEA17A-D745-4C2D-8DD3-2C789FAB878F}"/>
   </bookViews>
   <sheets>
     <sheet name="Table4" sheetId="1" r:id="rId1"/>
-    <sheet name="Cmax-stats" sheetId="2" r:id="rId2"/>
-    <sheet name="AUC-stats" sheetId="3" r:id="rId3"/>
+    <sheet name="main-stats-table" sheetId="4" r:id="rId2"/>
+    <sheet name="Cmax-stats" sheetId="2" r:id="rId3"/>
+    <sheet name="AUC-stats" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
   <si>
     <t>HTTK-InVitro</t>
   </si>
@@ -117,6 +118,48 @@
   </si>
   <si>
     <t>RPE High</t>
+  </si>
+  <si>
+    <t>AAFE</t>
+  </si>
+  <si>
+    <t>MRPE</t>
+  </si>
+  <si>
+    <t>RMSLE.early</t>
+  </si>
+  <si>
+    <t>RMSLE.late</t>
+  </si>
+  <si>
+    <t>AAFE.early</t>
+  </si>
+  <si>
+    <t>AAFE.late</t>
+  </si>
+  <si>
+    <t>MRPE.early</t>
+  </si>
+  <si>
+    <t>MRPE.late</t>
+  </si>
+  <si>
+    <t>RMSLE.bychem</t>
+  </si>
+  <si>
+    <t>RMSLE.bychem.early</t>
+  </si>
+  <si>
+    <t>RMSLE.bychem.late</t>
+  </si>
+  <si>
+    <t>Full Time Course</t>
+  </si>
+  <si>
+    <t>mRMSLE.by.chem</t>
+  </si>
+  <si>
+    <t>mRMSLE.all.points</t>
   </si>
 </sst>
 </file>
@@ -172,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -200,11 +243,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
     <dxf>
       <font>
         <strike val="0"/>
@@ -287,7 +331,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -301,7 +345,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -315,7 +359,47 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -369,30 +453,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C3B9A44-A160-4D79-9ECA-F4DB125D595C}" name="Table1" displayName="Table1" ref="A2:I9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A2:I9" xr:uid="{11B79BB4-92C5-4E45-B49C-36F612E26D41}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{BD031A34-C3A7-4714-9D00-DFA26E2C2BD9}" name="Predictor" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C3B9A44-A160-4D79-9ECA-F4DB125D595C}" name="Table1" displayName="Table1" ref="A2:K10" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A2:K10" xr:uid="{11B79BB4-92C5-4E45-B49C-36F612E26D41}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{BD031A34-C3A7-4714-9D00-DFA26E2C2BD9}" name="Predictor" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{625CEBB3-B0ED-481F-AC16-700A74874C2B}" name="mRMSLE.by.chem" dataDxfId="9">
+      <calculatedColumnFormula>INDEX('main-stats-table'!$A$1:$H$13,11,MATCH($A3,'main-stats-table'!$A$1:$H$1,0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{ECC465F2-0ECF-4E77-86D1-0A2FF10232CE}" name="mRMSLE.all.points" dataDxfId="8">
+      <calculatedColumnFormula>INDEX('main-stats-table'!$A$1:$H$13,3,MATCH($A3,'main-stats-table'!$A$1:$H$1,0))</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="9" xr3:uid="{D543F40E-1476-473C-B143-9F8F98CAE0C9}" name="Column4" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{32A545F2-ADD7-49F3-BDD0-5F2703B53E3E}" name="Column3" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{32A545F2-ADD7-49F3-BDD0-5F2703B53E3E}" name="Column3" dataDxfId="0">
       <calculatedColumnFormula>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C263D5CE-964A-476D-AAAC-218A3F21D030}" name="Column2" dataDxfId="5">
+    <tableColumn id="7" xr3:uid="{C263D5CE-964A-476D-AAAC-218A3F21D030}" name="Column2" dataDxfId="6">
       <calculatedColumnFormula>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7F899C7B-A313-4367-9075-B3D7502E319D}" name="Column1" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{7F899C7B-A313-4367-9075-B3D7502E319D}" name="Column1" dataDxfId="5">
       <calculatedColumnFormula>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{996D6B90-055A-4D94-A874-98020F868AE0}" name="R2" dataDxfId="3">
+    <tableColumn id="2" xr3:uid="{996D6B90-055A-4D94-A874-98020F868AE0}" name="R2" dataDxfId="4">
       <calculatedColumnFormula>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F332C8C5-2DB9-4C72-99CB-A6B523C08711}" name="RMSE" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{F332C8C5-2DB9-4C72-99CB-A6B523C08711}" name="RMSE" dataDxfId="3">
       <calculatedColumnFormula>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{83A664CF-CB94-48E9-B931-140B55FFCD99}" name="R22" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{83A664CF-CB94-48E9-B931-140B55FFCD99}" name="R22" dataDxfId="2">
       <calculatedColumnFormula>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FC8770FC-F8E8-42B4-ADA8-3C323E5DBFC9}" name="R222" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{FC8770FC-F8E8-42B4-ADA8-3C323E5DBFC9}" name="R222" dataDxfId="1">
       <calculatedColumnFormula>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -697,463 +787,585 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5E5AE0-6A96-4F05-89BB-1660FC314176}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
       <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
       <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,11,MATCH("FitsToData",'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="C3" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,3,MATCH("FitsToData",'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>0.72</v>
+      </c>
+      <c r="D3" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH("FitsToData",'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="C3" s="9">
-        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH("FitsToData",'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="D3" s="9">
+        <v>0.875</v>
+      </c>
+      <c r="E3" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH("FitsToData",'Cmax-stats'!$A$2:$A$9,0),3)</f>
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="F3" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH("FitsToData",'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>-8.8999999999999996E-2</v>
-      </c>
-      <c r="E3" s="9">
+        <v>-4.5999999999999999E-2</v>
+      </c>
+      <c r="G3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.96099999999999997</v>
-      </c>
-      <c r="F3" s="9">
+        <v>0.91</v>
+      </c>
+      <c r="H3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.309</v>
-      </c>
-      <c r="G3" s="9">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="I3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>0.315</v>
-      </c>
-      <c r="H3" s="9">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="J3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="I3" s="9">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="K3" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH("FitsToData",'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>6.1800000000000001E-2</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+        <v>0.254</v>
+      </c>
       <c r="L3" s="4"/>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,11,MATCH($A4,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="C4" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,3,MATCH($A4,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D4" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.56699999999999995</v>
-      </c>
-      <c r="C4" s="9">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="E4" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="F4" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
+        <v>-4.0300000000000002E-2</v>
+      </c>
+      <c r="G4" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
+        <v>0.496</v>
+      </c>
+      <c r="H4" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I4" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
+        <v>4.04</v>
+      </c>
+      <c r="J4" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
+        <v>7.52</v>
+      </c>
+      <c r="K4" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
+        <v>-0.41899999999999998</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$I$13,11,MATCH($A5,'main-stats-table'!$A$1:$I$1,0))</f>
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="C5" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$I$13,3,MATCH($A5,'main-stats-table'!$A$1:$I$1,0))</f>
+        <v>1.29</v>
+      </c>
+      <c r="D5" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="E5" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="F5" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
+        <v>8.8300000000000003E-2</v>
+      </c>
+      <c r="G5" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
+        <v>0.62</v>
+      </c>
+      <c r="H5" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
+        <v>1.06</v>
+      </c>
+      <c r="I5" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
+        <v>6.34</v>
+      </c>
+      <c r="J5" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
+        <v>10.5</v>
+      </c>
+      <c r="K5" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
+        <v>-0.154</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,11,MATCH($A6,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>1.03</v>
+      </c>
+      <c r="C6" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,3,MATCH($A6,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>1.08</v>
+      </c>
+      <c r="D6" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="E6" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="F6" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="G6" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="H6" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="I6" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
+        <v>5.52</v>
+      </c>
+      <c r="J6" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
+        <v>9.6</v>
+      </c>
+      <c r="K6" s="9">
+        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
+        <v>-0.45100000000000001</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,11,MATCH($A7,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="C7" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,3,MATCH($A7,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D7" s="9">
+        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="E7" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
         <v>0.83599999999999997</v>
       </c>
-      <c r="D4" s="9">
+      <c r="F7" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>-2.29E-2</v>
-      </c>
-      <c r="E4" s="9">
+        <v>-4.9300000000000004E-3</v>
+      </c>
+      <c r="G7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.495</v>
-      </c>
-      <c r="F4" s="9">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>3.44</v>
-      </c>
-      <c r="H4" s="9">
+        <v>3.37</v>
+      </c>
+      <c r="J7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>6.72</v>
-      </c>
-      <c r="I4" s="9">
+        <v>4.91</v>
+      </c>
+      <c r="K7" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.46400000000000002</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="9">
+        <v>-5.1799999999999999E-2</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,11,MATCH($A8,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>0.94</v>
+      </c>
+      <c r="C8" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,3,MATCH($A8,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D8" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.621</v>
-      </c>
-      <c r="C5" s="9">
+        <v>0.54</v>
+      </c>
+      <c r="E8" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="D5" s="9">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="F8" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>0.15</v>
-      </c>
-      <c r="E5" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="F5" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.96599999999999997</v>
-      </c>
-      <c r="G5" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>5.88</v>
-      </c>
-      <c r="H5" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>10.5</v>
-      </c>
-      <c r="I5" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.437</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="9">
-        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="C6" s="9">
-        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="D6" s="9">
-        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>1.6899999999999998E-2</v>
-      </c>
-      <c r="E6" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.58399999999999996</v>
-      </c>
-      <c r="F6" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.01</v>
-      </c>
-      <c r="G6" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>3.32</v>
-      </c>
-      <c r="H6" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>5</v>
-      </c>
-      <c r="I6" s="9">
-        <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-3.8199999999999998E-2</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="9">
-        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="C7" s="9">
-        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="D7" s="9">
-        <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>-0.105</v>
-      </c>
-      <c r="E7" s="9">
+        <v>-0.13800000000000001</v>
+      </c>
+      <c r="G8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
         <v>0.39600000000000002</v>
       </c>
-      <c r="F7" s="9">
+      <c r="H8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.22</v>
-      </c>
-      <c r="G7" s="9">
+        <v>1.21</v>
+      </c>
+      <c r="I8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>2.29</v>
-      </c>
-      <c r="H7" s="9">
+        <v>2.52</v>
+      </c>
+      <c r="J8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>5.99</v>
-      </c>
-      <c r="I7" s="9">
+        <v>6.34</v>
+      </c>
+      <c r="K8" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.79600000000000004</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+        <v>-0.78100000000000003</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B9" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,11,MATCH($A9,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="C9" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,3,MATCH($A9,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="D9" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="C8" s="9">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="E9" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.82599999999999996</v>
-      </c>
-      <c r="D8" s="9">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="F9" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>0.111</v>
-      </c>
-      <c r="E8" s="9">
+        <v>8.09E-2</v>
+      </c>
+      <c r="G9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F8" s="9">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="H9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.04</v>
-      </c>
-      <c r="G8" s="9">
+        <v>1.03</v>
+      </c>
+      <c r="I9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>4.67</v>
-      </c>
-      <c r="H8" s="9">
+        <v>4.68</v>
+      </c>
+      <c r="J9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>7.93</v>
-      </c>
-      <c r="I8" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="K9" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B10" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,11,MATCH($A10,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C10" s="9">
+        <f>INDEX('main-stats-table'!$A$1:$H$13,3,MATCH($A10,'main-stats-table'!$A$1:$H$1,0))</f>
+        <v>1.29</v>
+      </c>
+      <c r="D10" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="C9" s="9">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="E10" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),3)</f>
-        <v>0.93</v>
-      </c>
-      <c r="D9" s="9">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="F10" s="9">
         <f>INDEX('Cmax-stats'!$A$2:$D$9,MATCH(Table1[[#This Row],[Predictor]],'Cmax-stats'!$A$2:$A$9,0),4)</f>
-        <v>0.53100000000000003</v>
-      </c>
-      <c r="E9" s="9">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="G10" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),2)</f>
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="F9" s="9">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="H10" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),3)</f>
-        <v>1.48</v>
-      </c>
-      <c r="G9" s="9">
+        <v>1.38</v>
+      </c>
+      <c r="I10" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),4)</f>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="H9" s="9">
+        <v>6.12</v>
+      </c>
+      <c r="J10" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),5)</f>
-        <v>12.1</v>
-      </c>
-      <c r="I9" s="9">
+        <v>12.6</v>
+      </c>
+      <c r="K10" s="9">
         <f>INDEX('AUC-stats'!$A$2:$F$9,MATCH(Table1[[#This Row],[Predictor]],'AUC-stats'!$A$2:$A$9,0),6)</f>
-        <v>-0.88100000000000001</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+        <v>-0.86499999999999999</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F12" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G12" t="s">
         <v>6</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H12" t="s">
         <v>19</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I12" t="s">
         <v>20</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J12" t="s">
         <v>25</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K12" t="s">
         <v>26</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
       <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
       <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I17" s="1"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="7:13" x14ac:dyDescent="0.25">
-      <c r="M21" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="O22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1165,11 +1377,400 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F682B7B-67C2-4F10-B0D4-BA5227337A1C}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>7.15</v>
+      </c>
+      <c r="C2">
+        <v>6.49</v>
+      </c>
+      <c r="D2">
+        <v>6.59</v>
+      </c>
+      <c r="E2">
+        <v>7.04</v>
+      </c>
+      <c r="F2">
+        <v>6.77</v>
+      </c>
+      <c r="G2">
+        <v>2.88</v>
+      </c>
+      <c r="H2">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="I2">
+        <v>8.7799999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C3">
+        <v>1.08</v>
+      </c>
+      <c r="D3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F3">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.72</v>
+      </c>
+      <c r="H3">
+        <v>1.29</v>
+      </c>
+      <c r="I3">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>0.99</v>
+      </c>
+      <c r="C4">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D4">
+        <v>1.01</v>
+      </c>
+      <c r="E4">
+        <v>0.52</v>
+      </c>
+      <c r="F4">
+        <v>1.18</v>
+      </c>
+      <c r="G4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H4">
+        <v>1.17</v>
+      </c>
+      <c r="I4">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>1.04</v>
+      </c>
+      <c r="C5">
+        <v>0.94</v>
+      </c>
+      <c r="D5">
+        <v>1.01</v>
+      </c>
+      <c r="E5">
+        <v>1.07</v>
+      </c>
+      <c r="F5">
+        <v>1.03</v>
+      </c>
+      <c r="G5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H5">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="I5">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>1.38</v>
+      </c>
+      <c r="C6">
+        <v>1.32</v>
+      </c>
+      <c r="D6">
+        <v>1.3</v>
+      </c>
+      <c r="E6">
+        <v>1.29</v>
+      </c>
+      <c r="F6">
+        <v>1.36</v>
+      </c>
+      <c r="G6">
+        <v>0.94</v>
+      </c>
+      <c r="H6">
+        <v>1.6</v>
+      </c>
+      <c r="I6">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>5.62</v>
+      </c>
+      <c r="C7">
+        <v>4.74</v>
+      </c>
+      <c r="D7">
+        <v>5.3</v>
+      </c>
+      <c r="E7">
+        <v>5.9</v>
+      </c>
+      <c r="F7">
+        <v>5.35</v>
+      </c>
+      <c r="G7">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="H7">
+        <v>6.9</v>
+      </c>
+      <c r="I7">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>11.95</v>
+      </c>
+      <c r="C8">
+        <v>12.62</v>
+      </c>
+      <c r="D8">
+        <v>10.47</v>
+      </c>
+      <c r="E8">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="F8">
+        <v>11.17</v>
+      </c>
+      <c r="G8">
+        <v>4.54</v>
+      </c>
+      <c r="H8">
+        <v>20.12</v>
+      </c>
+      <c r="I8">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>0.52</v>
+      </c>
+      <c r="C9">
+        <v>0.47</v>
+      </c>
+      <c r="D9">
+        <v>0.49</v>
+      </c>
+      <c r="E9">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F9">
+        <v>0.6</v>
+      </c>
+      <c r="G9">
+        <v>0.3</v>
+      </c>
+      <c r="H9">
+        <v>0.48</v>
+      </c>
+      <c r="I9">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>3.62</v>
+      </c>
+      <c r="C10">
+        <v>6.11</v>
+      </c>
+      <c r="D10">
+        <v>3.25</v>
+      </c>
+      <c r="E10">
+        <v>1.93</v>
+      </c>
+      <c r="F10">
+        <v>3.67</v>
+      </c>
+      <c r="G10">
+        <v>1.84</v>
+      </c>
+      <c r="H10">
+        <v>8.61</v>
+      </c>
+      <c r="I10">
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="C11">
+        <v>1.03</v>
+      </c>
+      <c r="D11">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="E11">
+        <v>0.94</v>
+      </c>
+      <c r="F11">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="G11">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="H11">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.89600000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="D12">
+        <v>0.75</v>
+      </c>
+      <c r="E12">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="F12">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="I12">
+        <v>0.81200000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>1.08</v>
+      </c>
+      <c r="C13">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="E13">
+        <v>1.06</v>
+      </c>
+      <c r="F13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="H13">
+        <v>1.42</v>
+      </c>
+      <c r="I13">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29AF21A3-F045-4D6E-946A-E6C2D0038CF3}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,13 +1794,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.56699999999999995</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="C2">
-        <v>0.83599999999999997</v>
+        <v>0.86399999999999999</v>
       </c>
       <c r="D2">
-        <v>-2.29E-2</v>
+        <v>-4.0300000000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1207,13 +1808,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.621</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="C3">
-        <v>0.78200000000000003</v>
+        <v>0.81399999999999995</v>
       </c>
       <c r="D3">
-        <v>0.15</v>
+        <v>0.11799999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,13 +1822,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.59599999999999997</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="C4">
-        <v>0.80800000000000005</v>
+        <v>0.83599999999999997</v>
       </c>
       <c r="D4">
-        <v>1.6899999999999998E-2</v>
+        <v>-4.9300000000000004E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1235,13 +1836,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.56999999999999995</v>
+        <v>0.54</v>
       </c>
       <c r="C5">
-        <v>0.83299999999999996</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="D5">
-        <v>-0.105</v>
+        <v>-0.13800000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1249,13 +1850,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.57799999999999996</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="C6">
-        <v>0.82599999999999996</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="D6">
-        <v>0.111</v>
+        <v>8.09E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1263,13 +1864,13 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.94699999999999995</v>
+        <v>0.875</v>
       </c>
       <c r="C7">
-        <v>0.29399999999999998</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="D7">
-        <v>-8.8999999999999996E-2</v>
+        <v>-4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1277,13 +1878,13 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0.46400000000000002</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="C8">
-        <v>0.93</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="D8">
-        <v>0.53100000000000003</v>
+        <v>0.20100000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1291,13 +1892,13 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>0.60399999999999998</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="C9">
-        <v>0.86399999999999999</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="D9">
-        <v>0.156</v>
+        <v>8.8300000000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1305,12 +1906,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0089BC2-251A-4C09-B1F4-89BA489CD7D8}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,19 +1941,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.495</v>
+        <v>0.496</v>
       </c>
       <c r="C2">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D2">
-        <v>3.44</v>
+        <v>4.04</v>
       </c>
       <c r="E2">
-        <v>6.72</v>
+        <v>7.52</v>
       </c>
       <c r="F2">
-        <v>-0.46400000000000002</v>
+        <v>-0.41899999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1360,19 +1961,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.61799999999999999</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="C3">
-        <v>0.96599999999999997</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="D3">
-        <v>5.88</v>
+        <v>5.52</v>
       </c>
       <c r="E3">
-        <v>10.5</v>
+        <v>9.6</v>
       </c>
       <c r="F3">
-        <v>-0.437</v>
+        <v>-0.45100000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1380,19 +1981,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.58399999999999996</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="C4">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>3.32</v>
+        <v>3.37</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>4.91</v>
       </c>
       <c r="F4">
-        <v>-3.8199999999999998E-2</v>
+        <v>-5.1799999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1403,16 +2004,16 @@
         <v>0.39600000000000002</v>
       </c>
       <c r="C5">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
       <c r="D5">
-        <v>2.29</v>
+        <v>2.52</v>
       </c>
       <c r="E5">
-        <v>5.99</v>
+        <v>6.34</v>
       </c>
       <c r="F5">
-        <v>-0.79600000000000004</v>
+        <v>-0.78100000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1420,19 +2021,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.56000000000000005</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="C6">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
       <c r="D6">
-        <v>4.67</v>
+        <v>4.68</v>
       </c>
       <c r="E6">
-        <v>7.93</v>
+        <v>7.5</v>
       </c>
       <c r="F6">
-        <v>0.38500000000000001</v>
+        <v>0.31900000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1440,19 +2041,19 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.96099999999999997</v>
+        <v>0.91</v>
       </c>
       <c r="C7">
-        <v>0.309</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="D7">
-        <v>0.315</v>
+        <v>0.48399999999999999</v>
       </c>
       <c r="E7">
-        <v>0.41099999999999998</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="F7">
-        <v>6.1800000000000001E-2</v>
+        <v>0.254</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1460,19 +2061,19 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0.10199999999999999</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="C8">
-        <v>1.48</v>
+        <v>1.38</v>
       </c>
       <c r="D8">
-        <v>5.0999999999999996</v>
+        <v>6.12</v>
       </c>
       <c r="E8">
-        <v>12.1</v>
+        <v>12.6</v>
       </c>
       <c r="F8">
-        <v>-0.88100000000000001</v>
+        <v>-0.86499999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1480,19 +2081,19 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>0.622</v>
+        <v>0.62</v>
       </c>
       <c r="C9">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
       <c r="D9">
-        <v>4.6500000000000004</v>
+        <v>6.34</v>
       </c>
       <c r="E9">
         <v>10.5</v>
       </c>
       <c r="F9">
-        <v>-0.11799999999999999</v>
+        <v>-0.154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>